<commit_message>
Parece que la posicion del player ya esta bien, pero el mapa esta deformado
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MomentumEngine-Real\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MCV\MomentumEngine-Real\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Image pos</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>mushroom_kingdom_teleport</t>
+  </si>
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>Nestor pure arena</t>
   </si>
 </sst>
 </file>
@@ -52,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -92,10 +98,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,20 +385,28 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
       <c r="F1" t="s">
         <v>5</v>
       </c>
@@ -415,62 +429,62 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>169.78700000000001</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>-128.655</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>-325</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>-277.39999999999998</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f>SQRT(SUMXMY2(B3:C3,D3:E3))</f>
         <v>516.66164014178571</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>575</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>527</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>543</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>675</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>SQRT(SUMXMY2(B4:C4,D4:E4))</f>
         <v>151.4199458459816</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="F5">
         <f>F3/F4</f>
         <v>3.4121108500944359</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F6">
@@ -479,20 +493,68 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="B8">
+        <v>612.5</v>
+      </c>
+      <c r="C8">
+        <v>532.5</v>
+      </c>
+      <c r="D8">
+        <v>287</v>
+      </c>
+      <c r="E8">
+        <v>344</v>
+      </c>
+      <c r="F8">
+        <f>SQRT(SUMXMY2(B8:C8,D8:E8))</f>
+        <v>376.14159567907404</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>150.5</v>
+      </c>
+      <c r="C9">
+        <v>-146.5</v>
+      </c>
+      <c r="D9">
+        <v>-22</v>
+      </c>
+      <c r="E9">
+        <v>171.25</v>
+      </c>
+      <c r="F9">
+        <f>SQRT(SUMXMY2(B9:C9,D9:E9))</f>
+        <v>361.55402431725196</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
+      <c r="F11">
+        <f>F9/F8</f>
+        <v>0.96121787239327749</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
+      <c r="F12">
+        <f>F8/F9</f>
+        <v>1.0403468648685872</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
Se muestra bien la posicion del player en el mapa
</commit_message>
<xml_diff>
--- a/Map.xlsx
+++ b/Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Image pos</t>
   </si>
@@ -51,6 +51,24 @@
   </si>
   <si>
     <t>Nestor pure arena</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>bottom</t>
+  </si>
+  <si>
+    <t>tutorial</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>origin</t>
   </si>
 </sst>
 </file>
@@ -60,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +88,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +121,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,11 +597,98 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>-253.38</v>
+      </c>
+      <c r="C18">
+        <v>-0.501</v>
+      </c>
+      <c r="D18">
+        <v>316.06</v>
+      </c>
+      <c r="E18">
+        <v>155.179</v>
+      </c>
+      <c r="F18">
+        <v>-116.193</v>
+      </c>
+      <c r="G18">
+        <v>-367.024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>456</v>
+      </c>
+      <c r="C19">
+        <v>94</v>
+      </c>
+      <c r="D19">
+        <v>623</v>
+      </c>
+      <c r="E19">
+        <v>705</v>
+      </c>
+      <c r="F19">
+        <v>63</v>
+      </c>
+      <c r="G19">
+        <v>241</v>
+      </c>
+      <c r="I19">
+        <v>456</v>
+      </c>
+      <c r="J19">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F22" s="2">
+        <f>SQRT(SUMXMY2(B18:C18,D18:E18))</f>
+        <v>590.337340848434</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="2">
+        <f>SQRT(SUMXMY2(B19:C19,D19:E19))</f>
+        <v>633.41139869756057</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f>F22/F23</f>
+        <v>0.93199671187209965</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F25" s="4">
+        <f>F23/F22</f>
+        <v>1.0729651588483637</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>